<commit_message>
Grouping T&TG for H; filtering out M
</commit_message>
<xml_diff>
--- a/pH_measurement.xlsx
+++ b/pH_measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebec\Documents\Rebecca\UCU\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCED984F-0660-4093-ACCF-206E46E2C72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD59EFFD-96C2-4BDB-9B1F-B7962A3893D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C4E58CFA-B5CE-4363-AAAB-E3B42D498D6E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="169">
   <si>
     <t>Tube_ID</t>
   </si>
@@ -198,9 +198,6 @@
     <t>DV_H_R_05</t>
   </si>
   <si>
-    <t xml:space="preserve"> KD_B_R_02</t>
-  </si>
-  <si>
     <t>BK_B_T_05</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>SB_B_TG_04</t>
   </si>
   <si>
-    <t>Iron</t>
-  </si>
-  <si>
     <t>LM_B_T_05</t>
   </si>
   <si>
@@ -405,10 +399,148 @@
     <t>SV_B_TG_03</t>
   </si>
   <si>
-    <t>iron</t>
-  </si>
-  <si>
-    <t>CHECK</t>
+    <t>AS_H_T_03</t>
+  </si>
+  <si>
+    <t>VV_B_M_01</t>
+  </si>
+  <si>
+    <t>Error; half 0-10cm (in bag)</t>
+  </si>
+  <si>
+    <t>VV_B_M_02</t>
+  </si>
+  <si>
+    <t>VV_B_M_03</t>
+  </si>
+  <si>
+    <t>KD_B_R_05</t>
+  </si>
+  <si>
+    <t>BK_B_TG_02</t>
+  </si>
+  <si>
+    <t>BK_B_TG_03</t>
+  </si>
+  <si>
+    <t>BK_B_TG_01</t>
+  </si>
+  <si>
+    <t>BK_B_TG_05</t>
+  </si>
+  <si>
+    <t>SB_B_TG_03</t>
+  </si>
+  <si>
+    <t>SB_B_TG_05</t>
+  </si>
+  <si>
+    <t>WZ_B_TG_03</t>
+  </si>
+  <si>
+    <t>Barely enough; used bigger pieces because soil was very tough</t>
+  </si>
+  <si>
+    <t>BM_B_R_01</t>
+  </si>
+  <si>
+    <t>BH_B_TG_04</t>
+  </si>
+  <si>
+    <t>Very tough, left a piece in the bag</t>
+  </si>
+  <si>
+    <t>SH_B_T_01</t>
+  </si>
+  <si>
+    <t>SM_B_M_04</t>
+  </si>
+  <si>
+    <t>Very tough, used big pieces</t>
+  </si>
+  <si>
+    <t>SM_B_M_05</t>
+  </si>
+  <si>
+    <t>LS_B_R_02</t>
+  </si>
+  <si>
+    <t>LS_B_R_04</t>
+  </si>
+  <si>
+    <t>LM_B_T_02</t>
+  </si>
+  <si>
+    <t>HB_B_TG_02</t>
+  </si>
+  <si>
+    <t>BK_B_R_01</t>
+  </si>
+  <si>
+    <t>BK_B_R_05</t>
+  </si>
+  <si>
+    <t>GP_B_T_01</t>
+  </si>
+  <si>
+    <t>GP_B_T_03</t>
+  </si>
+  <si>
+    <t>VV_B_M_05</t>
+  </si>
+  <si>
+    <t>KD_B_R_02</t>
+  </si>
+  <si>
+    <t>Very tough, big chunks</t>
+  </si>
+  <si>
+    <t>BK_B_TG2_03</t>
+  </si>
+  <si>
+    <t>HB_B_TG_05</t>
+  </si>
+  <si>
+    <t>WZ_B_TG_02</t>
+  </si>
+  <si>
+    <t>WZ_B_TG_05</t>
+  </si>
+  <si>
+    <t>WW_B_R_03</t>
+  </si>
+  <si>
+    <t>BK_B_R_04</t>
+  </si>
+  <si>
+    <t>5g instead of 10g, not enough soil. Still used 25mL, otherwise the suspension was too thick</t>
+  </si>
+  <si>
+    <t>5g instead of 10g, not enough soil. Still used 25mL, otherwise the suspension was too thick; still very thick suspension</t>
+  </si>
+  <si>
+    <t>BM_B_R_03</t>
+  </si>
+  <si>
+    <t>BM_B_R_04</t>
+  </si>
+  <si>
+    <t>WZ_B_TG_04</t>
+  </si>
+  <si>
+    <t>9.8 g, not enough soil</t>
+  </si>
+  <si>
+    <t>GP_B_T_02</t>
+  </si>
+  <si>
+    <t>GP_B_T_04</t>
+  </si>
+  <si>
+    <t>AA_H_T_05</t>
+  </si>
+  <si>
+    <t>SD_H_T_04</t>
   </si>
 </sst>
 </file>
@@ -761,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9493FC-AB5C-4F2A-99B1-11654AB6A34D}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="D302" sqref="D302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1567,7 +1699,7 @@
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1581,7 +1713,7 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1595,7 +1727,7 @@
         <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1609,7 +1741,7 @@
         <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1623,7 +1755,7 @@
         <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1637,7 +1769,7 @@
         <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1651,7 +1783,7 @@
         <v>22</v>
       </c>
       <c r="B63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1665,7 +1797,7 @@
         <v>23</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1679,7 +1811,7 @@
         <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1693,7 +1825,7 @@
         <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1707,7 +1839,7 @@
         <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -1721,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1735,7 +1867,7 @@
         <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -1749,7 +1881,7 @@
         <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1763,7 +1895,7 @@
         <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -1791,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1805,7 +1937,7 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1819,7 +1951,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -1833,7 +1965,7 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -1842,7 +1974,7 @@
         <v>5.5</v>
       </c>
       <c r="E76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -1878,7 +2010,7 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -1887,7 +2019,7 @@
         <v>6.19</v>
       </c>
       <c r="E79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -1895,7 +2027,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -1909,7 +2041,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -1923,7 +2055,7 @@
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1937,7 +2069,7 @@
         <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1951,7 +2083,7 @@
         <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -1965,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -1979,7 +2111,7 @@
         <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -1993,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2007,7 +2139,7 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2021,7 +2153,7 @@
         <v>18</v>
       </c>
       <c r="B89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -2035,7 +2167,7 @@
         <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2044,7 +2176,7 @@
         <v>4.43</v>
       </c>
       <c r="E90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
@@ -2052,7 +2184,7 @@
         <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2066,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -2080,7 +2212,7 @@
         <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -2094,7 +2226,7 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2108,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -2122,7 +2254,7 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2136,16 +2268,13 @@
         <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
         <v>6.15</v>
-      </c>
-      <c r="E97" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -2153,16 +2282,13 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98" s="1">
         <v>6.48</v>
-      </c>
-      <c r="E98" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
@@ -2170,7 +2296,7 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -2212,7 +2338,7 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -2226,7 +2352,7 @@
         <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -2240,7 +2366,7 @@
         <v>13</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2249,7 +2375,7 @@
         <v>4.88</v>
       </c>
       <c r="E104" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -2257,7 +2383,7 @@
         <v>14</v>
       </c>
       <c r="B105" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -2271,7 +2397,7 @@
         <v>15</v>
       </c>
       <c r="B106" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2285,7 +2411,7 @@
         <v>16</v>
       </c>
       <c r="B107" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -2299,7 +2425,7 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -2313,7 +2439,7 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2327,7 +2453,7 @@
         <v>19</v>
       </c>
       <c r="B110" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2341,7 +2467,7 @@
         <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2355,7 +2481,7 @@
         <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2383,7 +2509,7 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2397,7 +2523,7 @@
         <v>24</v>
       </c>
       <c r="B115" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2411,7 +2537,7 @@
         <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2425,7 +2551,7 @@
         <v>26</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -2439,7 +2565,7 @@
         <v>27</v>
       </c>
       <c r="B118" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -2523,7 +2649,7 @@
         <v>3</v>
       </c>
       <c r="B124" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -2551,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="B126" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -2565,7 +2691,7 @@
         <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -2593,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="B129" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -2607,7 +2733,7 @@
         <v>9</v>
       </c>
       <c r="B130" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2621,7 +2747,7 @@
         <v>10</v>
       </c>
       <c r="B131" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2635,7 +2761,7 @@
         <v>11</v>
       </c>
       <c r="B132" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -2649,7 +2775,7 @@
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2663,7 +2789,7 @@
         <v>13</v>
       </c>
       <c r="B134" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -2677,7 +2803,7 @@
         <v>14</v>
       </c>
       <c r="B135" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2691,7 +2817,7 @@
         <v>15</v>
       </c>
       <c r="B136" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2705,7 +2831,7 @@
         <v>16</v>
       </c>
       <c r="B137" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -2719,7 +2845,7 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -2789,7 +2915,7 @@
         <v>22</v>
       </c>
       <c r="B143" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -2803,7 +2929,7 @@
         <v>23</v>
       </c>
       <c r="B144" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -2817,7 +2943,7 @@
         <v>24</v>
       </c>
       <c r="B145" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -2831,16 +2957,13 @@
         <v>25</v>
       </c>
       <c r="B146" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C146">
         <v>0</v>
       </c>
       <c r="D146" s="1">
         <v>5.12</v>
-      </c>
-      <c r="E146" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
@@ -2848,16 +2971,13 @@
         <v>26</v>
       </c>
       <c r="B147" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C147">
         <v>0</v>
       </c>
       <c r="D147" s="1">
         <v>5.6</v>
-      </c>
-      <c r="E147" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
@@ -2865,7 +2985,7 @@
         <v>27</v>
       </c>
       <c r="B148" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -2879,7 +2999,7 @@
         <v>28</v>
       </c>
       <c r="B149" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -2893,16 +3013,13 @@
         <v>29</v>
       </c>
       <c r="B150" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C150">
         <v>0</v>
       </c>
       <c r="D150" s="1">
         <v>5.53</v>
-      </c>
-      <c r="E150" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
@@ -2910,7 +3027,7 @@
         <v>30</v>
       </c>
       <c r="B151" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2919,7 +3036,7 @@
         <v>6.74</v>
       </c>
       <c r="E151" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
@@ -2927,16 +3044,13 @@
         <v>31</v>
       </c>
       <c r="B152" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C152">
         <v>0</v>
       </c>
       <c r="D152" s="1">
         <v>5.96</v>
-      </c>
-      <c r="E152" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
@@ -2944,13 +3058,13 @@
         <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C153">
         <v>0</v>
       </c>
-      <c r="E153" t="s">
-        <v>92</v>
+      <c r="D153" s="1">
+        <v>6.2</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -2958,13 +3072,13 @@
         <v>33</v>
       </c>
       <c r="B154" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C154">
         <v>0</v>
       </c>
-      <c r="E154" t="s">
-        <v>92</v>
+      <c r="D154" s="1">
+        <v>5.14</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
@@ -2972,10 +3086,13 @@
         <v>34</v>
       </c>
       <c r="B155" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C155">
         <v>1</v>
+      </c>
+      <c r="D155" s="1">
+        <v>6.52</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
@@ -2983,10 +3100,2088 @@
         <v>35</v>
       </c>
       <c r="B156" t="s">
+        <v>109</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156" s="1">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157" t="s">
+        <v>34</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157" s="1">
+        <v>5.1100000000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>2</v>
+      </c>
+      <c r="B158" t="s">
+        <v>121</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158" s="1">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>27</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159" s="1">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>4</v>
+      </c>
+      <c r="B160" t="s">
+        <v>122</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160" s="1">
+        <v>8.11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>122</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="D161" s="1">
+        <v>8.24</v>
+      </c>
+      <c r="E161" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>6</v>
+      </c>
+      <c r="B162" t="s">
+        <v>124</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162" s="1">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>124</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163" s="1">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>8</v>
+      </c>
+      <c r="B164" t="s">
+        <v>125</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164" s="1">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>9</v>
+      </c>
+      <c r="B165" t="s">
+        <v>125</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="D165" s="1">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>10</v>
+      </c>
+      <c r="B166" t="s">
+        <v>37</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166" s="1">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>11</v>
+      </c>
+      <c r="B167" t="s">
+        <v>126</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>12</v>
+      </c>
+      <c r="B168" t="s">
+        <v>50</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168" s="1">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>13</v>
+      </c>
+      <c r="B169" t="s">
+        <v>127</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169" s="1">
+        <v>7.27</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>14</v>
+      </c>
+      <c r="B170" t="s">
+        <v>128</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170" s="1">
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>15</v>
+      </c>
+      <c r="B171" t="s">
+        <v>129</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171" s="1">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>16</v>
+      </c>
+      <c r="B172" t="s">
+        <v>130</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172" s="1">
+        <v>7.93</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>17</v>
+      </c>
+      <c r="B173" t="s">
+        <v>115</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173" s="1">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>18</v>
+      </c>
+      <c r="B174" t="s">
+        <v>64</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174" s="1">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>19</v>
+      </c>
+      <c r="B175" t="s">
+        <v>43</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175" s="1">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>20</v>
+      </c>
+      <c r="B176" t="s">
+        <v>131</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176" s="1">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>21</v>
+      </c>
+      <c r="B177" t="s">
+        <v>131</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177" s="1">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>22</v>
+      </c>
+      <c r="B178" t="s">
+        <v>132</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178" s="1">
+        <v>6.23</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>23</v>
+      </c>
+      <c r="B179" t="s">
+        <v>132</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="D179" s="1">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>24</v>
+      </c>
+      <c r="B180" t="s">
+        <v>133</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180" s="1">
+        <v>6.17</v>
+      </c>
+      <c r="E180" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>25</v>
+      </c>
+      <c r="B181" t="s">
+        <v>96</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181" s="1">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>1</v>
+      </c>
+      <c r="B182" t="s">
+        <v>135</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182" s="1">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>2</v>
+      </c>
+      <c r="B183" t="s">
+        <v>135</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183" s="1">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>136</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184" s="1">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>4</v>
+      </c>
+      <c r="B185" t="s">
+        <v>95</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185" s="1">
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>5</v>
+      </c>
+      <c r="B186" t="s">
+        <v>61</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186" s="1">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>6</v>
+      </c>
+      <c r="B187" t="s">
+        <v>54</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187" s="1">
+        <v>7.03</v>
+      </c>
+      <c r="E187" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>7</v>
+      </c>
+      <c r="B188" t="s">
+        <v>138</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188" s="1">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>8</v>
+      </c>
+      <c r="B189" t="s">
+        <v>88</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189" s="1">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>9</v>
+      </c>
+      <c r="B190" t="s">
+        <v>89</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>10</v>
+      </c>
+      <c r="B191" t="s">
+        <v>87</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191" s="1">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>11</v>
+      </c>
+      <c r="B192" t="s">
+        <v>139</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E192" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>12</v>
+      </c>
+      <c r="B193" t="s">
+        <v>82</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+      <c r="D193" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E193" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>13</v>
+      </c>
+      <c r="B194" t="s">
+        <v>141</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194" s="1">
+        <v>4.55</v>
+      </c>
+      <c r="E194" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>14</v>
+      </c>
+      <c r="B195" t="s">
+        <v>98</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>15</v>
+      </c>
+      <c r="B196" t="s">
+        <v>66</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196" s="1">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>16</v>
+      </c>
+      <c r="B197" t="s">
+        <v>142</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197" s="1">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>17</v>
+      </c>
+      <c r="B198" t="s">
+        <v>142</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198" s="1">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>18</v>
+      </c>
+      <c r="B199" t="s">
+        <v>67</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>19</v>
+      </c>
+      <c r="B200" t="s">
+        <v>143</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+      <c r="D200" s="1">
+        <v>4.78</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>20</v>
+      </c>
+      <c r="B201" t="s">
+        <v>143</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201" s="1">
+        <v>4.96</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>21</v>
+      </c>
+      <c r="B202" t="s">
+        <v>144</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202" s="1">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>22</v>
+      </c>
+      <c r="B203" t="s">
+        <v>91</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203" s="1">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>23</v>
+      </c>
+      <c r="B204" t="s">
+        <v>145</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204" s="1">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>24</v>
+      </c>
+      <c r="B205" t="s">
+        <v>79</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205" s="1">
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>25</v>
+      </c>
+      <c r="B206" t="s">
+        <v>80</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206" s="1">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>26</v>
+      </c>
+      <c r="B207" t="s">
+        <v>127</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+      <c r="D207" s="1">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>27</v>
+      </c>
+      <c r="B208" t="s">
+        <v>128</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+      <c r="D208" s="1">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>28</v>
+      </c>
+      <c r="B209" t="s">
+        <v>130</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+      <c r="D209" s="1">
+        <v>8.15</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>29</v>
+      </c>
+      <c r="B210" t="s">
+        <v>146</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210" s="1">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>30</v>
+      </c>
+      <c r="B211" t="s">
+        <v>85</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+      <c r="D211" s="1">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>31</v>
+      </c>
+      <c r="B212" t="s">
+        <v>147</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+      <c r="D212" s="1">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>32</v>
+      </c>
+      <c r="B213" t="s">
+        <v>147</v>
+      </c>
+      <c r="C213">
+        <v>1</v>
+      </c>
+      <c r="D213" s="1">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>33</v>
+      </c>
+      <c r="B214" t="s">
+        <v>148</v>
+      </c>
+      <c r="C214">
+        <v>0</v>
+      </c>
+      <c r="D214" s="1">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>34</v>
+      </c>
+      <c r="B215" t="s">
+        <v>149</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215" s="1">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>35</v>
+      </c>
+      <c r="B216" t="s">
+        <v>149</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216" s="1">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>1</v>
+      </c>
+      <c r="B217" t="s">
+        <v>150</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+      <c r="D217" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>2</v>
+      </c>
+      <c r="B218" t="s">
+        <v>150</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+      <c r="D218" s="1">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>3</v>
+      </c>
+      <c r="B219" t="s">
+        <v>78</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219" s="1">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>4</v>
+      </c>
+      <c r="B220" t="s">
+        <v>97</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+      <c r="D220" s="1">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>5</v>
+      </c>
+      <c r="B221" t="s">
+        <v>151</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+      <c r="D221" s="1">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>6</v>
+      </c>
+      <c r="B222" t="s">
+        <v>126</v>
+      </c>
+      <c r="C222">
+        <v>0</v>
+      </c>
+      <c r="D222" s="1">
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>7</v>
+      </c>
+      <c r="B223" t="s">
+        <v>69</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="E223" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>8</v>
+      </c>
+      <c r="B224" t="s">
+        <v>136</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="D224" s="1">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>9</v>
+      </c>
+      <c r="B225" t="s">
+        <v>30</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225" s="1">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>10</v>
+      </c>
+      <c r="B226" t="s">
+        <v>62</v>
+      </c>
+      <c r="C226">
+        <v>0</v>
+      </c>
+      <c r="D226" s="1">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>11</v>
+      </c>
+      <c r="B227" t="s">
+        <v>153</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+      <c r="D227" s="1">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>12</v>
+      </c>
+      <c r="B228" t="s">
+        <v>153</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+      <c r="D228" s="1">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>13</v>
+      </c>
+      <c r="B229" t="s">
+        <v>114</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229" s="1">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>14</v>
+      </c>
+      <c r="B230" t="s">
+        <v>93</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230" s="1">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>15</v>
+      </c>
+      <c r="B231" t="s">
+        <v>51</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+      <c r="D231" s="1">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>16</v>
+      </c>
+      <c r="B232" t="s">
         <v>111</v>
       </c>
-      <c r="C156">
-        <v>1</v>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>17</v>
+      </c>
+      <c r="B233" t="s">
+        <v>41</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
+      </c>
+      <c r="D233" s="1">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>18</v>
+      </c>
+      <c r="B234" t="s">
+        <v>154</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234" s="1">
+        <v>7.76</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>19</v>
+      </c>
+      <c r="B235" t="s">
+        <v>154</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235" s="1">
+        <v>8.0299999999999994</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>20</v>
+      </c>
+      <c r="B236" t="s">
+        <v>145</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+      <c r="D236" s="1">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>21</v>
+      </c>
+      <c r="B237" t="s">
+        <v>49</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237" s="1">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A238">
+        <v>22</v>
+      </c>
+      <c r="B238" t="s">
+        <v>70</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238" s="1">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A239">
+        <v>23</v>
+      </c>
+      <c r="B239" t="s">
+        <v>94</v>
+      </c>
+      <c r="C239">
+        <v>1</v>
+      </c>
+      <c r="D239" s="1">
+        <v>7.04</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>24</v>
+      </c>
+      <c r="B240" t="s">
+        <v>133</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" s="1">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>25</v>
+      </c>
+      <c r="B241" t="s">
+        <v>155</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241" s="1">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A242">
+        <v>26</v>
+      </c>
+      <c r="B242" t="s">
+        <v>155</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+      <c r="D242" s="1">
+        <v>5.86</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A243">
+        <v>27</v>
+      </c>
+      <c r="B243" t="s">
+        <v>156</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+      <c r="D243" s="1">
+        <v>5.33</v>
+      </c>
+      <c r="E243" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A244">
+        <v>28</v>
+      </c>
+      <c r="B244" t="s">
+        <v>157</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+      <c r="D244" s="1">
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A245">
+        <v>29</v>
+      </c>
+      <c r="B245" t="s">
+        <v>157</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245" s="1">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A246">
+        <v>30</v>
+      </c>
+      <c r="B246" t="s">
+        <v>118</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+      <c r="D246" s="1">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A247">
+        <v>31</v>
+      </c>
+      <c r="B247" t="s">
+        <v>48</v>
+      </c>
+      <c r="C247">
+        <v>0</v>
+      </c>
+      <c r="D247" s="1">
+        <v>5.07</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A248">
+        <v>32</v>
+      </c>
+      <c r="B248" t="s">
+        <v>59</v>
+      </c>
+      <c r="C248">
+        <v>0</v>
+      </c>
+      <c r="D248" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A249">
+        <v>33</v>
+      </c>
+      <c r="B249" t="s">
+        <v>158</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249" s="1">
+        <v>6.73</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A250">
+        <v>34</v>
+      </c>
+      <c r="B250" t="s">
+        <v>129</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250" s="1">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A251">
+        <v>35</v>
+      </c>
+      <c r="B251" t="s">
+        <v>156</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251" s="1">
+        <v>5.51</v>
+      </c>
+      <c r="E251" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A252">
+        <v>1</v>
+      </c>
+      <c r="B252" t="s">
+        <v>117</v>
+      </c>
+      <c r="C252">
+        <v>0</v>
+      </c>
+      <c r="D252" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="E252" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A253">
+        <v>2</v>
+      </c>
+      <c r="B253" t="s">
+        <v>141</v>
+      </c>
+      <c r="C253">
+        <v>0</v>
+      </c>
+      <c r="D253" s="1">
+        <v>4.71</v>
+      </c>
+      <c r="E253" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A254">
+        <v>3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>116</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
+      <c r="D254" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="E254" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A255">
+        <v>4</v>
+      </c>
+      <c r="B255" t="s">
+        <v>139</v>
+      </c>
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255" s="1">
+        <v>4.59</v>
+      </c>
+      <c r="E255" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A256">
+        <v>5</v>
+      </c>
+      <c r="B256" t="s">
+        <v>146</v>
+      </c>
+      <c r="C256">
+        <v>0</v>
+      </c>
+      <c r="D256" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A257">
+        <v>6</v>
+      </c>
+      <c r="B257" t="s">
+        <v>144</v>
+      </c>
+      <c r="C257">
+        <v>0</v>
+      </c>
+      <c r="D257" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A258">
+        <v>7</v>
+      </c>
+      <c r="B258" t="s">
+        <v>113</v>
+      </c>
+      <c r="C258">
+        <v>1</v>
+      </c>
+      <c r="D258" s="1">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A259">
+        <v>8</v>
+      </c>
+      <c r="B259" t="s">
+        <v>86</v>
+      </c>
+      <c r="C259">
+        <v>0</v>
+      </c>
+      <c r="D259" s="1">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A260">
+        <v>9</v>
+      </c>
+      <c r="B260" t="s">
+        <v>158</v>
+      </c>
+      <c r="C260">
+        <v>0</v>
+      </c>
+      <c r="D260" s="1">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A261">
+        <v>10</v>
+      </c>
+      <c r="B261" t="s">
+        <v>45</v>
+      </c>
+      <c r="C261">
+        <v>0</v>
+      </c>
+      <c r="D261" s="1">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A262">
+        <v>11</v>
+      </c>
+      <c r="B262" t="s">
+        <v>161</v>
+      </c>
+      <c r="C262">
+        <v>0</v>
+      </c>
+      <c r="D262" s="1">
+        <v>5.55</v>
+      </c>
+      <c r="E262" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A263">
+        <v>12</v>
+      </c>
+      <c r="B263" t="s">
+        <v>161</v>
+      </c>
+      <c r="C263">
+        <v>1</v>
+      </c>
+      <c r="D263" s="1">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A264">
+        <v>13</v>
+      </c>
+      <c r="B264" t="s">
+        <v>162</v>
+      </c>
+      <c r="C264">
+        <v>1</v>
+      </c>
+      <c r="D264" s="1">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A265">
+        <v>14</v>
+      </c>
+      <c r="B265" t="s">
+        <v>162</v>
+      </c>
+      <c r="C265">
+        <v>0</v>
+      </c>
+      <c r="D265" s="1">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A266">
+        <v>15</v>
+      </c>
+      <c r="B266" t="s">
+        <v>163</v>
+      </c>
+      <c r="C266">
+        <v>0</v>
+      </c>
+      <c r="D266" s="1">
+        <v>5.89</v>
+      </c>
+      <c r="E266" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A267">
+        <v>16</v>
+      </c>
+      <c r="B267" t="s">
+        <v>163</v>
+      </c>
+      <c r="C267">
+        <v>1</v>
+      </c>
+      <c r="D267" s="1">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A268">
+        <v>17</v>
+      </c>
+      <c r="B268" t="s">
+        <v>138</v>
+      </c>
+      <c r="C268">
+        <v>0</v>
+      </c>
+      <c r="D268" s="1">
+        <v>5.54</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A269">
+        <v>18</v>
+      </c>
+      <c r="B269" t="s">
+        <v>46</v>
+      </c>
+      <c r="C269">
+        <v>1</v>
+      </c>
+      <c r="D269" s="1">
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A270">
+        <v>19</v>
+      </c>
+      <c r="B270" t="s">
+        <v>75</v>
+      </c>
+      <c r="C270">
+        <v>1</v>
+      </c>
+      <c r="D270" s="1">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A271">
+        <v>20</v>
+      </c>
+      <c r="B271" t="s">
+        <v>120</v>
+      </c>
+      <c r="C271">
+        <v>1</v>
+      </c>
+      <c r="D271" s="1">
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A272">
+        <v>21</v>
+      </c>
+      <c r="B272" t="s">
+        <v>102</v>
+      </c>
+      <c r="C272">
+        <v>0</v>
+      </c>
+      <c r="D272" s="1">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A273">
+        <v>22</v>
+      </c>
+      <c r="B273" t="s">
+        <v>92</v>
+      </c>
+      <c r="C273">
+        <v>0</v>
+      </c>
+      <c r="D273" s="1">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A274">
+        <v>23</v>
+      </c>
+      <c r="B274" t="s">
+        <v>60</v>
+      </c>
+      <c r="C274">
+        <v>1</v>
+      </c>
+      <c r="D274" s="1">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A275">
+        <v>24</v>
+      </c>
+      <c r="B275" t="s">
+        <v>148</v>
+      </c>
+      <c r="C275">
+        <v>1</v>
+      </c>
+      <c r="D275" s="1">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>25</v>
+      </c>
+      <c r="B276" t="s">
+        <v>165</v>
+      </c>
+      <c r="C276">
+        <v>1</v>
+      </c>
+      <c r="D276" s="1">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>26</v>
+      </c>
+      <c r="B277" t="s">
+        <v>165</v>
+      </c>
+      <c r="C277">
+        <v>0</v>
+      </c>
+      <c r="D277" s="1">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>27</v>
+      </c>
+      <c r="B278" t="s">
+        <v>166</v>
+      </c>
+      <c r="C278">
+        <v>0</v>
+      </c>
+      <c r="D278" s="1">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>28</v>
+      </c>
+      <c r="B279" t="s">
+        <v>166</v>
+      </c>
+      <c r="C279">
+        <v>1</v>
+      </c>
+      <c r="D279" s="1">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A280">
+        <v>1</v>
+      </c>
+      <c r="B280" t="s">
+        <v>36</v>
+      </c>
+      <c r="C280">
+        <v>0</v>
+      </c>
+      <c r="D280" s="1">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A281">
+        <v>2</v>
+      </c>
+      <c r="B281" t="s">
+        <v>121</v>
+      </c>
+      <c r="C281">
+        <v>0</v>
+      </c>
+      <c r="D281" s="1">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A282">
+        <v>3</v>
+      </c>
+      <c r="B282" t="s">
+        <v>5</v>
+      </c>
+      <c r="C282">
+        <v>0</v>
+      </c>
+      <c r="D282" s="1">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A283">
+        <v>4</v>
+      </c>
+      <c r="B283" t="s">
+        <v>167</v>
+      </c>
+      <c r="C283">
+        <v>0</v>
+      </c>
+      <c r="D283" s="1">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A284">
+        <v>5</v>
+      </c>
+      <c r="B284" t="s">
+        <v>167</v>
+      </c>
+      <c r="C284">
+        <v>1</v>
+      </c>
+      <c r="D284" s="1">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A285">
+        <v>6</v>
+      </c>
+      <c r="B285" t="s">
+        <v>32</v>
+      </c>
+      <c r="C285">
+        <v>1</v>
+      </c>
+      <c r="D285" s="1">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A286">
+        <v>7</v>
+      </c>
+      <c r="B286" t="s">
+        <v>13</v>
+      </c>
+      <c r="C286">
+        <v>1</v>
+      </c>
+      <c r="D286" s="1">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A287">
+        <v>8</v>
+      </c>
+      <c r="B287" t="s">
+        <v>100</v>
+      </c>
+      <c r="C287">
+        <v>1</v>
+      </c>
+      <c r="D287" s="1">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A288">
+        <v>9</v>
+      </c>
+      <c r="B288" t="s">
+        <v>101</v>
+      </c>
+      <c r="C288">
+        <v>1</v>
+      </c>
+      <c r="D288" s="1">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A289">
+        <v>10</v>
+      </c>
+      <c r="B289" t="s">
+        <v>105</v>
+      </c>
+      <c r="C289">
+        <v>1</v>
+      </c>
+      <c r="D289" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A290">
+        <v>11</v>
+      </c>
+      <c r="B290" t="s">
+        <v>53</v>
+      </c>
+      <c r="C290">
+        <v>1</v>
+      </c>
+      <c r="D290" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A291">
+        <v>12</v>
+      </c>
+      <c r="B291" t="s">
+        <v>29</v>
+      </c>
+      <c r="C291">
+        <v>0</v>
+      </c>
+      <c r="D291" s="1">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A292">
+        <v>13</v>
+      </c>
+      <c r="B292" t="s">
+        <v>12</v>
+      </c>
+      <c r="C292">
+        <v>0</v>
+      </c>
+      <c r="D292" s="1">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A293">
+        <v>14</v>
+      </c>
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293">
+        <v>0</v>
+      </c>
+      <c r="D293" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A294">
+        <v>15</v>
+      </c>
+      <c r="B294" t="s">
+        <v>57</v>
+      </c>
+      <c r="C294">
+        <v>0</v>
+      </c>
+      <c r="D294" s="1">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A295">
+        <v>16</v>
+      </c>
+      <c r="B295" t="s">
+        <v>168</v>
+      </c>
+      <c r="C295">
+        <v>0</v>
+      </c>
+      <c r="D295" s="1">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A296">
+        <v>17</v>
+      </c>
+      <c r="B296" t="s">
+        <v>168</v>
+      </c>
+      <c r="C296">
+        <v>1</v>
+      </c>
+      <c r="D296" s="1">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A297">
+        <v>18</v>
+      </c>
+      <c r="B297" t="s">
+        <v>24</v>
+      </c>
+      <c r="C297">
+        <v>1</v>
+      </c>
+      <c r="D297" s="1">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A298">
+        <v>19</v>
+      </c>
+      <c r="B298" t="s">
+        <v>9</v>
+      </c>
+      <c r="C298">
+        <v>0</v>
+      </c>
+      <c r="D298" s="1">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A299">
+        <v>20</v>
+      </c>
+      <c r="B299" t="s">
+        <v>14</v>
+      </c>
+      <c r="C299">
+        <v>0</v>
+      </c>
+      <c r="D299" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A300">
+        <v>21</v>
+      </c>
+      <c r="B300" t="s">
+        <v>76</v>
+      </c>
+      <c r="C300">
+        <v>0</v>
+      </c>
+      <c r="D300" s="1">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A301">
+        <v>22</v>
+      </c>
+      <c r="B301" t="s">
+        <v>4</v>
+      </c>
+      <c r="C301">
+        <v>0</v>
+      </c>
+      <c r="D301" s="1">
+        <v>6.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>